<commit_message>
data opruimen (ik heb alle originele files behouden zodat we steeds alles kunnen checken mocht er twijfel zijn)
</commit_message>
<xml_diff>
--- a/Measurement_Results/UV-VIS/11.03.16/GNP_11032016_1.xlsx
+++ b/Measurement_Results/UV-VIS/11.03.16/GNP_11032016_1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="20730" windowHeight="9780"/>
+    <workbookView xWindow="0" yWindow="135" windowWidth="23955" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -332,8 +332,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -445,7 +445,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Tecan.At.Excel.Attenuation" xfId="6"/>
     <cellStyle name="Tecan.At.Excel.AutoGain_0" xfId="7"/>
     <cellStyle name="Tecan.At.Excel.Error" xfId="1"/>
@@ -456,18 +456,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -505,7 +500,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -539,7 +534,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -574,10 +568,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -750,16 +743,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:WD189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CF38" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:XFD45"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -767,7 +758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -778,7 +769,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -786,7 +777,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -794,7 +785,7 @@
         <v>42440</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -802,7 +793,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -810,7 +801,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -818,7 +809,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -826,17 +817,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -844,7 +835,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:602">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -855,7 +846,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:602">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -866,7 +857,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:602">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -877,7 +868,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:602">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -885,7 +876,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="21" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:602">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -893,7 +884,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:602">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -901,7 +892,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:602">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -909,7 +900,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:602">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -920,7 +911,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:602">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -928,7 +919,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:602">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -936,12 +927,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:602">
       <c r="B28" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:602">
       <c r="A29" s="3" t="s">
         <v>37</v>
       </c>
@@ -2749,67 +2740,67 @@
         <v>900</v>
       </c>
     </row>
-    <row r="30" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:602">
       <c r="A30" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:602">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:602">
       <c r="A32" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:602">
       <c r="A33" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:602">
       <c r="A34" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:602">
       <c r="A35" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:602">
       <c r="A36" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:602">
       <c r="A37" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:602">
       <c r="A38" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:602">
       <c r="A39" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:602">
       <c r="A40" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:602">
       <c r="A41" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:602">
       <c r="A42" s="3" t="s">
         <v>50</v>
       </c>
@@ -4617,7 +4608,7 @@
         <v>0.1281999945640564</v>
       </c>
     </row>
-    <row r="43" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:602">
       <c r="A43" s="3" t="s">
         <v>51</v>
       </c>
@@ -6425,7 +6416,7 @@
         <v>0.15360000729560852</v>
       </c>
     </row>
-    <row r="44" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:602">
       <c r="A44" s="3" t="s">
         <v>52</v>
       </c>
@@ -8233,7 +8224,7 @@
         <v>0.14069999754428864</v>
       </c>
     </row>
-    <row r="45" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:602">
       <c r="A45" s="3" t="s">
         <v>53</v>
       </c>
@@ -8715,97 +8706,97 @@
         <v>0.32969999313354492</v>
       </c>
     </row>
-    <row r="46" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:602">
       <c r="A46" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:602">
       <c r="A47" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:602">
       <c r="A48" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1">
       <c r="A50" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1">
       <c r="A51" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1">
       <c r="A52" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1">
       <c r="A53" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1">
       <c r="A54" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1">
       <c r="A55" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1">
       <c r="A56" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1">
       <c r="A57" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1">
       <c r="A58" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1">
       <c r="A59" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1">
       <c r="A60" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1">
       <c r="A61" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1">
       <c r="A62" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1">
       <c r="A63" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:1">
       <c r="A189" t="s">
         <v>72</v>
       </c>
@@ -8817,12 +8808,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>